<commit_message>
ECP-780: adds project fixture for Italy
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/charge/fixtures/incoming/builders/CapexChargeHierarchy.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/charge/fixtures/incoming/builders/CapexChargeHierarchy.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
   <si>
     <t>PROJECT MANAGEMENT</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>FURNITURES / DECORATION</t>
+  </si>
+  <si>
+    <t>/ITA</t>
+  </si>
+  <si>
+    <t>PURCHASE</t>
+  </si>
+  <si>
+    <t>CONSTRUCTION</t>
   </si>
 </sst>
 </file>
@@ -479,7 +488,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -487,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z15"/>
+  <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -732,6 +741,22 @@
         <v>15</v>
       </c>
     </row>
+    <row r="16" spans="1:26" ht="15" customHeight="1">
+      <c r="A16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1">
+      <c r="A17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>

</xml_diff>

<commit_message>
EST-1862: adds createOrder, integtest for OrderMenu
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/charge/fixtures/incoming/builders/CapexChargeHierarchy.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/charge/fixtures/incoming/builders/CapexChargeHierarchy.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28028"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sander/src/bitbucket/incodehq/estatio-ecp/estatio/estatioapp/app/src/main/java/org/estatio/module/charge/fixtures/incoming/builders/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A926566D-073C-0B49-942F-0E832BE83475}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27880" windowHeight="12800"/>
+    <workbookView xWindow="5160" yWindow="-17260" windowWidth="27880" windowHeight="12800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChargeHierarchy" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -81,13 +87,13 @@
     <t>PURCHASE</t>
   </si>
   <si>
-    <t>CONSTRUCTION</t>
+    <t>ITWT001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -488,27 +494,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="38.5" customWidth="1"/>
     <col min="5" max="5" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -542,7 +548,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="14">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
@@ -574,7 +580,7 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:26" ht="14">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -588,7 +594,7 @@
       <c r="E3" s="5"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:26" ht="14">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -602,7 +608,7 @@
       <c r="E4" s="5"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:26" ht="14">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -616,7 +622,7 @@
       <c r="E5" s="5"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:26" ht="14">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -629,7 +635,7 @@
       <c r="D6" s="5"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:26" ht="14">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -643,7 +649,7 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:26" ht="14">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
@@ -656,7 +662,7 @@
       <c r="D8" s="5"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:26" ht="14">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -669,7 +675,7 @@
       <c r="D9" s="5"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:26" ht="14">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
@@ -682,7 +688,7 @@
       <c r="D10" s="5"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:26" ht="14">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -694,7 +700,7 @@
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:26" ht="14">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
@@ -706,7 +712,7 @@
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:26" ht="14">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -718,7 +724,7 @@
       </c>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:26" ht="15" customHeight="1">
+    <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
@@ -730,7 +736,7 @@
       </c>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:26" ht="15" customHeight="1">
+    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
@@ -741,7 +747,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="15" customHeight="1">
+    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
@@ -749,7 +755,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1">
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>

</xml_diff>